<commit_message>
82: Modify the production code of firmware version, old code about PGS7=0, from now PGS7=20. Named V0.36 (Date20250708)
</commit_message>
<xml_diff>
--- a/Objects/PGS7-0-36_202500704-BurnFile/PGS7_FW_ChangeNote.xlsx
+++ b/Objects/PGS7-0-36_202500704-BurnFile/PGS7_FW_ChangeNote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20917" windowHeight="9660"/>
+    <workbookView windowWidth="17017" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="PGS7" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t>当前版本</t>
   </si>
@@ -332,14 +332,6 @@
   </si>
   <si>
     <t>1：改善柳工测试ASC发现的一个异常。</t>
-  </si>
-  <si>
-    <t>PGS7-0-36_20250704-T5m</t>
-  </si>
-  <si>
-    <t>1：导入黄工修改的和Midea母板结合通信异常问题。
-2：改善一个取地址处理错问题。
-3：本固件适应硬件丝印PGS7000_V1.0。又称为PGS7000-E1或者E1-PGS7000.</t>
   </si>
 </sst>
 </file>
@@ -970,7 +962,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -981,9 +973,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1334,10 +1323,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1855,20 +1844,6 @@
       </c>
       <c r="D36" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="37" ht="54" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>